<commit_message>
Monthly report and TZA-4 extended to 12 elements. Tranliteration added to the file name...
</commit_message>
<xml_diff>
--- a/reports/monthly_templ.xlsx
+++ b/reports/monthly_templ.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t xml:space="preserve">Ежемесячный отчет</t>
   </si>
@@ -44,6 +44,7 @@
         <color rgb="FF00000A"/>
         <rFont val="Liberation Serif;Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">год</t>
     </r>
@@ -63,6 +64,7 @@
         <color rgb="FF00000A"/>
         <rFont val="Liberation Serif;Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">месяц</t>
     </r>
@@ -72,6 +74,7 @@
         <color rgb="FF00000A"/>
         <rFont val="Liberation Serif;Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">  {d[i].values[i].month}</t>
     </r>
@@ -89,6 +92,9 @@
     <t xml:space="preserve">NO2</t>
   </si>
   <si>
+    <t xml:space="preserve">NH3</t>
+  </si>
+  <si>
     <t xml:space="preserve">SO2</t>
   </si>
   <si>
@@ -101,10 +107,19 @@
     <t xml:space="preserve">CO</t>
   </si>
   <si>
+    <t xml:space="preserve">CH2O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM-2,5</t>
+  </si>
+  <si>
     <t xml:space="preserve">PM-10</t>
   </si>
   <si>
-    <t xml:space="preserve">PM-2,5</t>
+    <t xml:space="preserve">Пыль общая</t>
   </si>
   <si>
     <t xml:space="preserve">{d[i].values [i].pollution[i].time}</t>
@@ -116,6 +131,9 @@
     <t xml:space="preserve">{d[i].values [i].pollution[i].valueNO2}</t>
   </si>
   <si>
+    <t xml:space="preserve">{d[i].values [i].pollution[i].valueNH3}</t>
+  </si>
+  <si>
     <t xml:space="preserve">{d[i].values [i].pollution[i].valueSO2}</t>
   </si>
   <si>
@@ -128,10 +146,19 @@
     <t xml:space="preserve">{d[i].values [i].pollution[i].valueCO}</t>
   </si>
   <si>
+    <t xml:space="preserve">{d[i].values [i].pollution[i].valueCH2O}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d[i].values [i].pollution[i].valuePM1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d[i].values [i].pollution[i].valuePM25}</t>
+  </si>
+  <si>
     <t xml:space="preserve">{d[i].values [i].pollution[i].valuePM10}</t>
   </si>
   <si>
-    <t xml:space="preserve">{d[i].values [i].pollution[i].valuePM25}</t>
+    <t xml:space="preserve">{d[i].values [i].pollution[i].valueTSP}</t>
   </si>
   <si>
     <t xml:space="preserve">{d[i].values [i].pollution[i+1].time}</t>
@@ -147,6 +174,7 @@
         <color rgb="FF00000A"/>
         <rFont val="Liberation Serif;Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Контролируемые параметры:</t>
     </r>
@@ -156,9 +184,13 @@
         <color rgb="FF00000A"/>
         <rFont val="Liberation Serif;Times New Roman"/>
         <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> NO — оксид азота, NO2 -двуокись азота, SO2 — диоксид серы, О3 — озон, СО — угарный газ, РМ-10 — твердые частицы 10 мкм, PM-2,5 - твердые частицы 2,5 мкм.</t>
-    </r>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> NO — оксид азота, NO2 -двуокись азота, NH3 - аммиак, SO2 — диоксид серы, О3 — озон, СО — угарный газ, CH2O - формальдегид, </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">РМ-1 — твердые частицы 1 мкм, PM-2,5 - твердые частицы 2,5 мкм, РМ-10 — твердые частицы 10 мкм, Пыль общая — твердые частицы все фракции.</t>
   </si>
   <si>
     <r>
@@ -168,6 +200,7 @@
         <color rgb="FF00000A"/>
         <rFont val="Liberation Serif;Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Метеопараметры:</t>
     </r>
@@ -177,6 +210,7 @@
         <color rgb="FF00000A"/>
         <rFont val="Liberation Serif;Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> давление — мм.рт.ст.; температура внешняя, внутренняя - °С; влажность внешняя, внутренняя — %; скорость ветра — м/с; направление ветра — градусы; осадки — мм.</t>
     </r>
@@ -204,7 +238,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -225,26 +259,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF00000A"/>
-      <name val="Liberation Serif;Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF00000A"/>
-      <name val="Liberation Serif;Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF00000A"/>
-      <name val="Liberation Serif;Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -255,11 +269,46 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF00000A"/>
+      <name val="Liberation Serif;Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00000A"/>
+      <name val="Liberation Serif;Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="7.2"/>
+      <color rgb="FF00000A"/>
+      <name val="Liberation Serif;Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="7.2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3C3C3C"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="9"/>
       <color rgb="FF00000A"/>
       <name val="Liberation Serif;Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -311,7 +360,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -328,31 +377,47 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -422,7 +487,7 @@
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF3C3C3C"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -433,17 +498,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="5:7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="2" style="0" width="12.1836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.48469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3010204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="2" style="0" width="11.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="7.86734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -458,6 +523,10 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -473,6 +542,10 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -488,6 +561,10 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
@@ -515,105 +592,140 @@
       <c r="I4" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="E5" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="42.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>24</v>
+      <c r="A8" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>25</v>
+        <v>31</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="20.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="42.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="5"/>
+      <c r="A13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="12"/>
       <c r="D13" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>27</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
-        <v>28</v>
+      <c r="A14" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>30</v>
+        <v>38</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="B2:M2"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B3:M3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.39375" right="0.39375" top="0.659027777777778" bottom="0.659027777777778" header="0.39375" footer="0.39375"/>

</xml_diff>

<commit_message>
Point of measure to reports added... Issues with point status fixed.
</commit_message>
<xml_diff>
--- a/reports/monthly_templ.xlsx
+++ b/reports/monthly_templ.xlsx
@@ -30,12 +30,40 @@
   <si>
     <r>
       <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Точка отбора: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{d[i].values[i].point} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">    </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -310,7 +338,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -335,6 +363,25 @@
     <font>
       <b val="true"/>
       <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
@@ -470,27 +517,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -498,15 +545,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -514,19 +565,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -534,15 +581,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -550,11 +597,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -638,13 +685,13 @@
   <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T13" activeCellId="0" sqref="T13"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="7.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="6" style="0" width="10.95"/>
   </cols>
   <sheetData>

</xml_diff>